<commit_message>
Ran code that created CAAR graphs
</commit_message>
<xml_diff>
--- a/data/final/graph_data.xlsx
+++ b/data/final/graph_data.xlsx
@@ -1292,7 +1292,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>40230.8</t>
+          <t>40230.800000000003</t>
         </is>
       </c>
       <c r="AD3" t="n">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>40387.27</t>
+          <t>40387.269999999997</t>
         </is>
       </c>
       <c r="AD4" t="n">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>605.2</t>
+          <t>605.20000000000005</t>
         </is>
       </c>
       <c r="AD5" t="n">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="AN13" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO13" t="n">
@@ -4388,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="AZ13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB13" t="n">
         <v>1</v>
@@ -7937,7 +7937,7 @@
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>-0.006</t>
+          <t>-6.0000000000000001E-3</t>
         </is>
       </c>
       <c r="AG25" t="n">
@@ -9426,7 +9426,7 @@
         <v>-11.09</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.833</v>
+        <v>0.8329999999999999</v>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
@@ -9730,7 +9730,7 @@
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>269.91</t>
+          <t>269.91000000000003</t>
         </is>
       </c>
       <c r="AD31" t="n">
@@ -10045,7 +10045,7 @@
       </c>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>0.698</t>
+          <t>0.69799999999999995</t>
         </is>
       </c>
       <c r="AG32" t="n">
@@ -10347,7 +10347,7 @@
       </c>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>2.03</t>
+          <t>2.0299999999999998</t>
         </is>
       </c>
       <c r="AG33" t="n">
@@ -11551,7 +11551,7 @@
       </c>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>0.267</t>
+          <t>0.26700000000000002</t>
         </is>
       </c>
       <c r="AG37" t="n">
@@ -12435,14 +12435,14 @@
         <v>1.28</v>
       </c>
       <c r="AA40" t="n">
-        <v>0.482</v>
+        <v>0.4819999999999999</v>
       </c>
       <c r="AB40" t="n">
         <v>2.69</v>
       </c>
       <c r="AC40" t="inlineStr">
         <is>
-          <t>38.12</t>
+          <t>38.119999999999997</t>
         </is>
       </c>
       <c r="AD40" t="n">
@@ -14250,7 +14250,7 @@
       </c>
       <c r="AC46" t="inlineStr">
         <is>
-          <t>2119.03</t>
+          <t>2119.0300000000002</t>
         </is>
       </c>
       <c r="AD46" t="n">
@@ -14550,7 +14550,7 @@
       </c>
       <c r="AC47" t="inlineStr">
         <is>
-          <t>2119.03</t>
+          <t>2119.0300000000002</t>
         </is>
       </c>
       <c r="AD47" t="n">
@@ -15150,7 +15150,7 @@
       </c>
       <c r="AC49" t="inlineStr">
         <is>
-          <t>35491.13</t>
+          <t>35491.129999999997</t>
         </is>
       </c>
       <c r="AD49" t="n">
@@ -15493,7 +15493,7 @@
       </c>
       <c r="AN50" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO50" t="n">
@@ -15530,10 +15530,10 @@
         <v>1</v>
       </c>
       <c r="AZ50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB50" t="n">
         <v>1</v>
@@ -18154,7 +18154,7 @@
       </c>
       <c r="AC59" t="inlineStr">
         <is>
-          <t>151.39</t>
+          <t>151.38999999999999</t>
         </is>
       </c>
       <c r="AD59" t="n">
@@ -18167,7 +18167,7 @@
       </c>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>0.8070000000000001</t>
+          <t>0.80700000000000005</t>
         </is>
       </c>
       <c r="AG59" t="n">
@@ -19671,7 +19671,7 @@
       </c>
       <c r="AF64" t="inlineStr">
         <is>
-          <t>317.96</t>
+          <t>317.95999999999998</t>
         </is>
       </c>
       <c r="AG64" t="n">
@@ -19956,7 +19956,7 @@
         <v>64.93000000000001</v>
       </c>
       <c r="AB65" t="n">
-        <v>0.118</v>
+        <v>0.1179999999999999</v>
       </c>
       <c r="AC65" t="inlineStr">
         <is>
@@ -20273,7 +20273,7 @@
       </c>
       <c r="AF66" t="inlineStr">
         <is>
-          <t>0.476</t>
+          <t>0.47599999999999998</t>
         </is>
       </c>
       <c r="AG66" t="n">
@@ -20603,7 +20603,7 @@
       </c>
       <c r="AN67" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO67" t="n">
@@ -20640,10 +20640,10 @@
         <v>0</v>
       </c>
       <c r="AZ67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB67" t="n">
         <v>1</v>
@@ -20864,7 +20864,7 @@
       </c>
       <c r="AC68" t="inlineStr">
         <is>
-          <t>319.04</t>
+          <t>319.04000000000002</t>
         </is>
       </c>
       <c r="AD68" t="n">
@@ -21464,7 +21464,7 @@
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>640.8200000000001</t>
+          <t>640.82000000000005</t>
         </is>
       </c>
       <c r="AD70" t="n">
@@ -21477,7 +21477,7 @@
       </c>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>0.334</t>
+          <t>0.33400000000000002</t>
         </is>
       </c>
       <c r="AG70" t="n">
@@ -22381,7 +22381,7 @@
       </c>
       <c r="AF73" t="inlineStr">
         <is>
-          <t>0.07099999999999999</t>
+          <t>7.0999999999999994E-2</t>
         </is>
       </c>
       <c r="AG73" t="n">
@@ -23274,7 +23274,7 @@
         </is>
       </c>
       <c r="AD76" t="n">
-        <v>79.59999999999999</v>
+        <v>79.59999999999998</v>
       </c>
       <c r="AE76" t="inlineStr">
         <is>
@@ -25091,7 +25091,7 @@
       </c>
       <c r="AF82" t="inlineStr">
         <is>
-          <t>-0.268</t>
+          <t>-0.26800000000000002</t>
         </is>
       </c>
       <c r="AG82" t="n">
@@ -26295,7 +26295,7 @@
       </c>
       <c r="AF86" t="inlineStr">
         <is>
-          <t>1093.85</t>
+          <t>1093.8499999999999</t>
         </is>
       </c>
       <c r="AG86" t="n">
@@ -26574,7 +26574,7 @@
         <v>34.56</v>
       </c>
       <c r="Z87" t="n">
-        <v>8.529999999999999</v>
+        <v>8.529999999999998</v>
       </c>
       <c r="AA87" t="n">
         <v>7.28</v>
@@ -26584,7 +26584,7 @@
       </c>
       <c r="AC87" t="inlineStr">
         <is>
-          <t>64.26000000000001</t>
+          <t>64.260000000000005</t>
         </is>
       </c>
       <c r="AD87" t="n">
@@ -26597,7 +26597,7 @@
       </c>
       <c r="AF87" t="inlineStr">
         <is>
-          <t>0.533</t>
+          <t>0.53300000000000003</t>
         </is>
       </c>
       <c r="AG87" t="n">
@@ -26899,7 +26899,7 @@
       </c>
       <c r="AF88" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.2999999999999998</t>
         </is>
       </c>
       <c r="AG88" t="n">
@@ -27201,7 +27201,7 @@
       </c>
       <c r="AF89" t="inlineStr">
         <is>
-          <t>0.061</t>
+          <t>6.0999999999999999E-2</t>
         </is>
       </c>
       <c r="AG89" t="n">
@@ -28431,7 +28431,7 @@
       </c>
       <c r="AN93" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO93" t="n">
@@ -28468,10 +28468,10 @@
         <v>1</v>
       </c>
       <c r="AZ93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB93" t="n">
         <v>1</v>
@@ -29007,7 +29007,7 @@
       </c>
       <c r="AF95" t="inlineStr">
         <is>
-          <t>0.703</t>
+          <t>0.70299999999999996</t>
         </is>
       </c>
       <c r="AG95" t="n">
@@ -31113,7 +31113,7 @@
       </c>
       <c r="AF102" t="inlineStr">
         <is>
-          <t>-0.269</t>
+          <t>-0.26900000000000002</t>
         </is>
       </c>
       <c r="AG102" t="n">
@@ -32297,7 +32297,7 @@
         <v>168.61</v>
       </c>
       <c r="AA106" t="n">
-        <v>75.56999999999999</v>
+        <v>75.56999999999998</v>
       </c>
       <c r="AB106" t="n">
         <v>114</v>
@@ -32647,7 +32647,7 @@
       </c>
       <c r="AN107" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO107" t="n">
@@ -32684,10 +32684,10 @@
         <v>1</v>
       </c>
       <c r="AZ107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB107" t="n">
         <v>1</v>
@@ -34712,7 +34712,7 @@
       </c>
       <c r="AC114" t="inlineStr">
         <is>
-          <t>38.27</t>
+          <t>38.270000000000003</t>
         </is>
       </c>
       <c r="AD114" t="n">
@@ -34725,7 +34725,7 @@
       </c>
       <c r="AF114" t="inlineStr">
         <is>
-          <t>0.059</t>
+          <t>5.8999999999999997E-2</t>
         </is>
       </c>
       <c r="AG114" t="n">
@@ -35929,7 +35929,7 @@
       </c>
       <c r="AF118" t="inlineStr">
         <is>
-          <t>17.49</t>
+          <t>17.489999999999998</t>
         </is>
       </c>
       <c r="AG118" t="n">
@@ -36822,7 +36822,7 @@
       </c>
       <c r="AC121" t="inlineStr">
         <is>
-          <t>2520.74</t>
+          <t>2520.7399999999998</t>
         </is>
       </c>
       <c r="AD121" t="n">
@@ -37424,7 +37424,7 @@
       </c>
       <c r="AC123" t="inlineStr">
         <is>
-          <t>87124.64999999999</t>
+          <t>87124.65</t>
         </is>
       </c>
       <c r="AD123" t="n">
@@ -38337,7 +38337,7 @@
       </c>
       <c r="AF126" t="inlineStr">
         <is>
-          <t>0.099</t>
+          <t>9.9000000000000005E-2</t>
         </is>
       </c>
       <c r="AG126" t="n">
@@ -38967,7 +38967,7 @@
       </c>
       <c r="AN128" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO128" t="n">
@@ -39004,10 +39004,10 @@
         <v>0</v>
       </c>
       <c r="AZ128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB128" t="n">
         <v>0</v>
@@ -39239,7 +39239,7 @@
       </c>
       <c r="AF129" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.84799999999999998</t>
         </is>
       </c>
       <c r="AG129" t="n">
@@ -39843,7 +39843,7 @@
       </c>
       <c r="AF131" t="inlineStr">
         <is>
-          <t>0.289</t>
+          <t>0.28899999999999998</t>
         </is>
       </c>
       <c r="AG131" t="n">
@@ -40174,7 +40174,7 @@
       </c>
       <c r="AN132" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO132" t="n">
@@ -40211,10 +40211,10 @@
         <v>0</v>
       </c>
       <c r="AZ132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB132" t="n">
         <v>1</v>
@@ -41050,7 +41050,7 @@
       </c>
       <c r="AF135" t="inlineStr">
         <is>
-          <t>0.091</t>
+          <t>9.0999999999999998E-2</t>
         </is>
       </c>
       <c r="AG135" t="n">
@@ -41940,7 +41940,7 @@
       </c>
       <c r="AC138" t="inlineStr">
         <is>
-          <t>65732.24000000001</t>
+          <t>65732.240000000005</t>
         </is>
       </c>
       <c r="AD138" t="n">
@@ -44063,7 +44063,7 @@
       </c>
       <c r="AF145" t="inlineStr">
         <is>
-          <t>0.029</t>
+          <t>2.9000000000000001E-2</t>
         </is>
       </c>
       <c r="AG145" t="n">
@@ -44665,7 +44665,7 @@
       </c>
       <c r="AF147" t="inlineStr">
         <is>
-          <t>-0.131</t>
+          <t>-0.13100000000000001</t>
         </is>
       </c>
       <c r="AG147" t="n">
@@ -46171,7 +46171,7 @@
       </c>
       <c r="AF152" t="inlineStr">
         <is>
-          <t>4.89</t>
+          <t>4.8899999999999997</t>
         </is>
       </c>
       <c r="AG152" t="n">
@@ -46773,7 +46773,7 @@
       </c>
       <c r="AF154" t="inlineStr">
         <is>
-          <t>0.273</t>
+          <t>0.27300000000000002</t>
         </is>
       </c>
       <c r="AG154" t="n">
@@ -47062,7 +47062,7 @@
       </c>
       <c r="AC155" t="inlineStr">
         <is>
-          <t>2244.57</t>
+          <t>2244.5700000000002</t>
         </is>
       </c>
       <c r="AD155" t="n">
@@ -47377,7 +47377,7 @@
       </c>
       <c r="AF156" t="inlineStr">
         <is>
-          <t>0.273</t>
+          <t>0.27300000000000002</t>
         </is>
       </c>
       <c r="AG156" t="n">
@@ -47979,7 +47979,7 @@
       </c>
       <c r="AF158" t="inlineStr">
         <is>
-          <t>2420.68</t>
+          <t>2420.6799999999998</t>
         </is>
       </c>
       <c r="AG158" t="n">
@@ -48268,7 +48268,7 @@
       </c>
       <c r="AC159" t="inlineStr">
         <is>
-          <t>512.8200000000001</t>
+          <t>512.82000000000005</t>
         </is>
       </c>
       <c r="AD159" t="n">
@@ -48570,7 +48570,7 @@
       </c>
       <c r="AC160" t="inlineStr">
         <is>
-          <t>848.3099999999999</t>
+          <t>848.31</t>
         </is>
       </c>
       <c r="AD160" t="n">
@@ -50076,7 +50076,7 @@
       </c>
       <c r="AC165" t="inlineStr">
         <is>
-          <t>2323.07</t>
+          <t>2323.0700000000002</t>
         </is>
       </c>
       <c r="AD165" t="n">
@@ -50976,7 +50976,7 @@
       </c>
       <c r="AC168" t="inlineStr">
         <is>
-          <t>4823.44</t>
+          <t>4823.4399999999996</t>
         </is>
       </c>
       <c r="AD168" t="n">
@@ -51017,7 +51017,7 @@
       </c>
       <c r="AN168" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO168" t="n">
@@ -51054,10 +51054,10 @@
         <v>1</v>
       </c>
       <c r="AZ168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB168" t="n">
         <v>1</v>
@@ -51276,7 +51276,7 @@
       </c>
       <c r="AC169" t="inlineStr">
         <is>
-          <t>2169.22</t>
+          <t>2169.2199999999998</t>
         </is>
       </c>
       <c r="AD169" t="n">
@@ -51317,7 +51317,7 @@
       </c>
       <c r="AN169" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO169" t="n">
@@ -51354,10 +51354,10 @@
         <v>1</v>
       </c>
       <c r="AZ169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA169" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB169" t="n">
         <v>1</v>
@@ -51578,7 +51578,7 @@
       </c>
       <c r="AC170" t="inlineStr">
         <is>
-          <t>39.55</t>
+          <t>39.549999999999997</t>
         </is>
       </c>
       <c r="AD170" t="n">
@@ -53072,7 +53072,7 @@
         <v>19.98</v>
       </c>
       <c r="Z175" t="n">
-        <v>0.093</v>
+        <v>0.09300000000000001</v>
       </c>
       <c r="AA175" t="n">
         <v>-0.279</v>
@@ -53102,7 +53102,7 @@
         <v>5.05</v>
       </c>
       <c r="AH175" t="n">
-        <v>0.713</v>
+        <v>0.7129999999999999</v>
       </c>
       <c r="AI175" t="inlineStr">
         <is>
@@ -53369,7 +53369,7 @@
         </is>
       </c>
       <c r="Y176" t="n">
-        <v>0.611</v>
+        <v>0.6109999999999999</v>
       </c>
       <c r="Z176" t="n">
         <v>-0.749</v>
@@ -54023,7 +54023,7 @@
       </c>
       <c r="AN178" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO178" t="n">
@@ -54060,10 +54060,10 @@
         <v>1</v>
       </c>
       <c r="AZ178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB178" t="n">
         <v>1</v>
@@ -54295,7 +54295,7 @@
       </c>
       <c r="AF179" t="inlineStr">
         <is>
-          <t>0.094</t>
+          <t>9.4E-2</t>
         </is>
       </c>
       <c r="AG179" t="n">
@@ -55484,7 +55484,7 @@
         <v>-230.01</v>
       </c>
       <c r="AB183" t="n">
-        <v>76.98999999999999</v>
+        <v>76.98999999999998</v>
       </c>
       <c r="AC183" t="inlineStr">
         <is>
@@ -55529,7 +55529,7 @@
       </c>
       <c r="AN183" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO183" t="n">
@@ -55566,10 +55566,10 @@
         <v>0</v>
       </c>
       <c r="AZ183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB183" t="n">
         <v>1</v>
@@ -55801,11 +55801,11 @@
       </c>
       <c r="AF184" t="inlineStr">
         <is>
-          <t>0.271</t>
+          <t>0.27100000000000002</t>
         </is>
       </c>
       <c r="AG184" t="n">
-        <v>9003.469999999999</v>
+        <v>9003.469999999998</v>
       </c>
       <c r="AH184" t="n">
         <v>277.62</v>
@@ -56980,7 +56980,7 @@
         <v>734.4400000000001</v>
       </c>
       <c r="Z188" t="n">
-        <v>75.48999999999999</v>
+        <v>75.48999999999998</v>
       </c>
       <c r="AA188" t="n">
         <v>21.87</v>
@@ -57892,7 +57892,7 @@
       </c>
       <c r="AC191" t="inlineStr">
         <is>
-          <t>262.71</t>
+          <t>262.70999999999998</t>
         </is>
       </c>
       <c r="AD191" t="n">
@@ -58805,7 +58805,7 @@
       </c>
       <c r="AF194" t="inlineStr">
         <is>
-          <t>0.658</t>
+          <t>0.65800000000000003</t>
         </is>
       </c>
       <c r="AG194" t="n">
@@ -59397,7 +59397,7 @@
       </c>
       <c r="AC196" t="inlineStr">
         <is>
-          <t>8.699999999999999</t>
+          <t>8.6999999999999993</t>
         </is>
       </c>
       <c r="AD196" t="n">
@@ -60010,7 +60010,7 @@
       </c>
       <c r="AF198" t="inlineStr">
         <is>
-          <t>0.645</t>
+          <t>0.64500000000000002</t>
         </is>
       </c>
       <c r="AG198" t="n">
@@ -60641,7 +60641,7 @@
       </c>
       <c r="AN200" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO200" t="n">
@@ -60678,10 +60678,10 @@
         <v>1</v>
       </c>
       <c r="AZ200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB200" t="n">
         <v>1</v>
@@ -61500,7 +61500,7 @@
       </c>
       <c r="AC203" t="inlineStr">
         <is>
-          <t>874.1900000000001</t>
+          <t>874.19</t>
         </is>
       </c>
       <c r="AD203" t="n">
@@ -61513,7 +61513,7 @@
       </c>
       <c r="AF203" t="inlineStr">
         <is>
-          <t>0.055</t>
+          <t>5.5E-2</t>
         </is>
       </c>
       <c r="AG203" t="n">
@@ -63599,7 +63599,7 @@
         <v>98.26000000000001</v>
       </c>
       <c r="Z210" t="n">
-        <v>0.425</v>
+        <v>0.4249999999999999</v>
       </c>
       <c r="AA210" t="n">
         <v>-18.55</v>
@@ -65398,7 +65398,7 @@
         </is>
       </c>
       <c r="Y216" t="n">
-        <v>0.351</v>
+        <v>0.3509999999999999</v>
       </c>
       <c r="Z216" t="n">
         <v>-5.13</v>
@@ -67237,7 +67237,7 @@
         <v>41.19</v>
       </c>
       <c r="AH222" t="n">
-        <v>0.286</v>
+        <v>0.2859999999999999</v>
       </c>
       <c r="AI222" t="inlineStr">
         <is>
@@ -67530,7 +67530,7 @@
       </c>
       <c r="AF223" t="inlineStr">
         <is>
-          <t>0.036</t>
+          <t>3.5999999999999997E-2</t>
         </is>
       </c>
       <c r="AG223" t="n">
@@ -68721,7 +68721,7 @@
       </c>
       <c r="AC227" t="inlineStr">
         <is>
-          <t>97.79000000000001</t>
+          <t>97.79</t>
         </is>
       </c>
       <c r="AD227" t="n">
@@ -69014,7 +69014,7 @@
         <v>1.21</v>
       </c>
       <c r="AA228" t="n">
-        <v>0.368</v>
+        <v>0.3679999999999999</v>
       </c>
       <c r="AB228" t="n">
         <v>4.6</v>
@@ -69321,7 +69321,7 @@
       </c>
       <c r="AC229" t="inlineStr">
         <is>
-          <t>613.2</t>
+          <t>613.20000000000005</t>
         </is>
       </c>
       <c r="AD229" t="n">
@@ -70521,7 +70521,7 @@
       </c>
       <c r="AC233" t="inlineStr">
         <is>
-          <t>1026.65</t>
+          <t>1026.6500000000001</t>
         </is>
       </c>
       <c r="AD233" t="n">
@@ -71134,7 +71134,7 @@
       </c>
       <c r="AF235" t="inlineStr">
         <is>
-          <t>-0.038</t>
+          <t>-3.7999999999999999E-2</t>
         </is>
       </c>
       <c r="AG235" t="n">
@@ -71423,7 +71423,7 @@
       </c>
       <c r="AC236" t="inlineStr">
         <is>
-          <t>5100.31</t>
+          <t>5100.3100000000004</t>
         </is>
       </c>
       <c r="AD236" t="n">
@@ -72316,7 +72316,7 @@
         <v>53.62</v>
       </c>
       <c r="Z239" t="n">
-        <v>-0.594</v>
+        <v>-0.5939999999999999</v>
       </c>
       <c r="AA239" t="n">
         <v>-33.38</v>
@@ -72628,7 +72628,7 @@
       </c>
       <c r="AC240" t="inlineStr">
         <is>
-          <t>147.95</t>
+          <t>147.94999999999999</t>
         </is>
       </c>
       <c r="AD240" t="n">
@@ -72928,7 +72928,7 @@
       </c>
       <c r="AC241" t="inlineStr">
         <is>
-          <t>4375.1</t>
+          <t>4375.1000000000004</t>
         </is>
       </c>
       <c r="AD241" t="n">
@@ -72941,7 +72941,7 @@
       </c>
       <c r="AF241" t="inlineStr">
         <is>
-          <t>75.90000000000001</t>
+          <t>75.900000000000006</t>
         </is>
       </c>
       <c r="AG241" t="n">
@@ -73227,7 +73227,7 @@
         <v>-2.84</v>
       </c>
       <c r="AB242" t="n">
-        <v>0.352</v>
+        <v>0.3519999999999999</v>
       </c>
       <c r="AC242" t="inlineStr">
         <is>
@@ -73828,7 +73828,7 @@
         <v>47.8</v>
       </c>
       <c r="AB244" t="n">
-        <v>74.73999999999999</v>
+        <v>74.73999999999998</v>
       </c>
       <c r="AC244" t="inlineStr">
         <is>
@@ -74434,7 +74434,7 @@
       </c>
       <c r="AC246" t="inlineStr">
         <is>
-          <t>17.35</t>
+          <t>17.350000000000001</t>
         </is>
       </c>
       <c r="AD246" t="n">
@@ -76554,7 +76554,7 @@
       </c>
       <c r="AF253" t="inlineStr">
         <is>
-          <t>-0.057</t>
+          <t>-5.7000000000000002E-2</t>
         </is>
       </c>
       <c r="AG253" t="n">
@@ -78947,7 +78947,7 @@
       </c>
       <c r="AC261" t="inlineStr">
         <is>
-          <t>2.18</t>
+          <t>2.1800000000000002</t>
         </is>
       </c>
       <c r="AD261" t="n">
@@ -79863,7 +79863,7 @@
       </c>
       <c r="AF264" t="inlineStr">
         <is>
-          <t>-0.035</t>
+          <t>-3.5000000000000003E-2</t>
         </is>
       </c>
       <c r="AG264" t="n">
@@ -80165,7 +80165,7 @@
       </c>
       <c r="AF265" t="inlineStr">
         <is>
-          <t>2.18</t>
+          <t>2.1800000000000002</t>
         </is>
       </c>
       <c r="AG265" t="n">
@@ -80754,7 +80754,7 @@
       </c>
       <c r="AC267" t="inlineStr">
         <is>
-          <t>17822.65</t>
+          <t>17822.650000000001</t>
         </is>
       </c>
       <c r="AD267" t="n">
@@ -81056,7 +81056,7 @@
       </c>
       <c r="AC268" t="inlineStr">
         <is>
-          <t>16.31</t>
+          <t>16.309999999999999</t>
         </is>
       </c>
       <c r="AD268" t="n">
@@ -81958,7 +81958,7 @@
       </c>
       <c r="AC271" t="inlineStr">
         <is>
-          <t>37695.41</t>
+          <t>37695.410000000003</t>
         </is>
       </c>
       <c r="AD271" t="n">
@@ -82258,7 +82258,7 @@
       </c>
       <c r="AC272" t="inlineStr">
         <is>
-          <t>666.1799999999999</t>
+          <t>666.18</t>
         </is>
       </c>
       <c r="AD272" t="n">
@@ -83202,7 +83202,7 @@
       </c>
       <c r="AN275" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
       <c r="AO275" t="n">
@@ -83239,10 +83239,10 @@
         <v>1</v>
       </c>
       <c r="AZ275" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA275" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB275" t="n">
         <v>1</v>
@@ -84361,7 +84361,7 @@
       </c>
       <c r="AC279" t="inlineStr">
         <is>
-          <t>4.85</t>
+          <t>4.8499999999999996</t>
         </is>
       </c>
       <c r="AD279" t="n">
@@ -85002,7 +85002,7 @@
       </c>
       <c r="AN281" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
       <c r="AO281" t="n">
@@ -85039,10 +85039,10 @@
         <v>1</v>
       </c>
       <c r="AZ281" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB281" t="n">
         <v>0</v>
@@ -85302,7 +85302,7 @@
       </c>
       <c r="AN282" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO282" t="n">
@@ -85339,10 +85339,10 @@
         <v>0</v>
       </c>
       <c r="AZ282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA282" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB282" t="n">
         <v>1</v>
@@ -86177,7 +86177,7 @@
       </c>
       <c r="AF285" t="inlineStr">
         <is>
-          <t>0.173</t>
+          <t>0.17299999999999999</t>
         </is>
       </c>
       <c r="AG285" t="n">
@@ -87068,7 +87068,7 @@
       </c>
       <c r="AC288" t="inlineStr">
         <is>
-          <t>90.73999999999999</t>
+          <t>90.74</t>
         </is>
       </c>
       <c r="AD288" t="n">
@@ -87409,7 +87409,7 @@
       </c>
       <c r="AN289" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
       <c r="AO289" t="n">
@@ -87446,10 +87446,10 @@
         <v>1</v>
       </c>
       <c r="AZ289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA289" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB289" t="n">
         <v>1</v>

</xml_diff>